<commit_message>
Finalizado automação para transferencia de arquivos entre computadores na rede !
</commit_message>
<xml_diff>
--- a/users_transfer.xlsx
+++ b/users_transfer.xlsx
@@ -1,50 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>COPIAR</t>
-  </si>
-  <si>
-    <t>COLAR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -59,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -96,34 +141,34 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -137,71 +182,69 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -225,53 +268,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -281,7 +325,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -290,7 +334,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -299,7 +343,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -307,10 +351,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -339,7 +383,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -352,12 +396,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -375,29 +420,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="16.719285714285714" customWidth="1" bestFit="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>COPIAR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>COLAR</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C:\Users\hospi\Favorites\TESTE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C:\Users\gabriel.oliveira\Favorites</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C:\Users\hospi\Favorites\TESTE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C:\Users\gabriel.oliveira\Favorites</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>